<commit_message>
CB invest policy V1.1
</commit_message>
<xml_diff>
--- a/CB/可转债交易数据.xlsx
+++ b/CB/可转债交易数据.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$44</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="99">
   <si>
     <t>转债代码</t>
   </si>
@@ -275,6 +275,45 @@
   </si>
   <si>
     <t>星帅转债</t>
+  </si>
+  <si>
+    <t>时达转债</t>
+  </si>
+  <si>
+    <t>机器人及</t>
+  </si>
+  <si>
+    <t>利群转债</t>
+  </si>
+  <si>
+    <t>商业零售</t>
+  </si>
+  <si>
+    <t>商场</t>
+  </si>
+  <si>
+    <t>众兴转债</t>
+  </si>
+  <si>
+    <t>农业</t>
+  </si>
+  <si>
+    <t>种植业</t>
+  </si>
+  <si>
+    <t>好客转债</t>
+  </si>
+  <si>
+    <t>维尔转债</t>
+  </si>
+  <si>
+    <t>长集转债</t>
+  </si>
+  <si>
+    <t>天路转债</t>
+  </si>
+  <si>
+    <t>水泥</t>
   </si>
 </sst>
 </file>
@@ -282,10 +321,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
   <fonts count="21">
@@ -306,7 +345,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -321,15 +382,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -337,28 +390,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -372,9 +403,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -442,8 +472,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -470,6 +509,72 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -482,7 +587,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,121 +665,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -632,25 +689,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -675,21 +714,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -776,6 +800,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -784,10 +823,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -796,137 +835,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -954,25 +993,10 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
@@ -1300,12 +1324,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1351,7 +1375,7 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
@@ -1369,7 +1393,7 @@
       <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="10" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1402,7 +1426,7 @@
         <f>(130-F2)*G2</f>
         <v>1199.95</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="11">
         <f>I2/H2</f>
         <v>0.226403524495052</v>
       </c>
@@ -1423,7 +1447,7 @@
         <f>N2-H2</f>
         <v>76.2299999999996</v>
       </c>
-      <c r="P2" s="14">
+      <c r="P2" s="11">
         <f>O2/H2</f>
         <v>0.0143828831803473</v>
       </c>
@@ -1454,11 +1478,11 @@
         <v>5015</v>
       </c>
       <c r="I3" s="5">
-        <f t="shared" ref="I3:I30" si="0">(130-F3)*G3</f>
+        <f t="shared" ref="I3:I38" si="0">(130-F3)*G3</f>
         <v>1485</v>
       </c>
-      <c r="J3" s="14">
-        <f t="shared" ref="J3:J30" si="1">I3/H3</f>
+      <c r="J3" s="11">
+        <f t="shared" ref="J3:J38" si="1">I3/H3</f>
         <v>0.296111665004985</v>
       </c>
       <c r="K3" s="5">
@@ -1477,7 +1501,7 @@
         <f>N3-H3</f>
         <v>2254.85</v>
       </c>
-      <c r="P3" s="14">
+      <c r="P3" s="11">
         <f>O3/H3</f>
         <v>0.449621136590229</v>
       </c>
@@ -1511,7 +1535,7 @@
         <f t="shared" si="0"/>
         <v>696</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="11">
         <f t="shared" si="1"/>
         <v>0.154529307282416</v>
       </c>
@@ -1520,7 +1544,7 @@
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
-      <c r="P4" s="15"/>
+      <c r="P4" s="12"/>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="7">
@@ -1551,7 +1575,7 @@
         <f t="shared" si="0"/>
         <v>720</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="11">
         <f t="shared" si="1"/>
         <v>0.160714285714286</v>
       </c>
@@ -1560,7 +1584,7 @@
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
-      <c r="P5" s="15"/>
+      <c r="P5" s="12"/>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="5">
@@ -1591,7 +1615,7 @@
         <f t="shared" si="0"/>
         <v>945</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="11">
         <f t="shared" si="1"/>
         <v>0.17011701170117</v>
       </c>
@@ -1611,7 +1635,7 @@
         <f>N6-H6</f>
         <v>945</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="11">
         <f>O6/H6</f>
         <v>0.17011701170117</v>
       </c>
@@ -1645,7 +1669,7 @@
         <f t="shared" si="0"/>
         <v>716.68</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="11">
         <f t="shared" si="1"/>
         <v>0.159854750497399</v>
       </c>
@@ -1654,7 +1678,7 @@
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
-      <c r="P7" s="15"/>
+      <c r="P7" s="12"/>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="7">
@@ -1685,7 +1709,7 @@
         <f t="shared" si="0"/>
         <v>883.5</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="11">
         <f t="shared" si="1"/>
         <v>0.157304371049586</v>
       </c>
@@ -1694,7 +1718,7 @@
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
-      <c r="P8" s="15"/>
+      <c r="P8" s="12"/>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="5">
@@ -1725,7 +1749,7 @@
         <f t="shared" si="0"/>
         <v>1045</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="11">
         <f t="shared" si="1"/>
         <v>0.191567369385885</v>
       </c>
@@ -1745,7 +1769,7 @@
         <f>N9-H9</f>
         <v>1046</v>
       </c>
-      <c r="P9" s="14">
+      <c r="P9" s="11">
         <f>O9/H9</f>
         <v>0.191750687442713</v>
       </c>
@@ -1779,7 +1803,7 @@
         <f t="shared" si="0"/>
         <v>905</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="11">
         <f t="shared" si="1"/>
         <v>0.161751563896336</v>
       </c>
@@ -1788,7 +1812,7 @@
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
-      <c r="P10" s="15"/>
+      <c r="P10" s="12"/>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="5">
@@ -1819,7 +1843,7 @@
         <f t="shared" si="0"/>
         <v>864</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="11">
         <f t="shared" si="1"/>
         <v>0.153300212916962</v>
       </c>
@@ -1839,7 +1863,7 @@
         <f>N11-H11</f>
         <v>864</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P11" s="11">
         <f>O11/H11</f>
         <v>0.153300212916962</v>
       </c>
@@ -1873,7 +1897,7 @@
         <f t="shared" si="0"/>
         <v>865</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="11">
         <f t="shared" si="1"/>
         <v>0.153504880212955</v>
       </c>
@@ -1894,7 +1918,7 @@
         <f>N12-H12</f>
         <v>987.499999999999</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P12" s="11">
         <f>O12/H12</f>
         <v>0.175244010647737</v>
       </c>
@@ -1928,7 +1952,7 @@
         <f t="shared" si="0"/>
         <v>1245</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="11">
         <f t="shared" si="1"/>
         <v>0.236917221693625</v>
       </c>
@@ -1948,7 +1972,7 @@
         <f>N13-H13</f>
         <v>1245</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13" s="11">
         <f>O13/H13</f>
         <v>0.236917221693625</v>
       </c>
@@ -1982,7 +2006,7 @@
         <f t="shared" si="0"/>
         <v>1190</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="11">
         <f t="shared" si="1"/>
         <v>0.224105461393597</v>
       </c>
@@ -1991,7 +2015,7 @@
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
-      <c r="P14" s="15"/>
+      <c r="P14" s="12"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="5">
@@ -2022,7 +2046,7 @@
         <f t="shared" si="0"/>
         <v>1205</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="11">
         <f t="shared" si="1"/>
         <v>0.227573182247403</v>
       </c>
@@ -2042,7 +2066,7 @@
         <f>N15-H15</f>
         <v>1205.05</v>
       </c>
-      <c r="P15" s="14">
+      <c r="P15" s="11">
         <f>O15/H15</f>
         <v>0.227582625118036</v>
       </c>
@@ -2076,7 +2100,7 @@
         <f t="shared" si="0"/>
         <v>1321.25</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="11">
         <f t="shared" si="1"/>
         <v>0.255129133478156</v>
       </c>
@@ -2085,7 +2109,7 @@
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
-      <c r="P16" s="15"/>
+      <c r="P16" s="12"/>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="5">
@@ -2116,7 +2140,7 @@
         <f t="shared" si="0"/>
         <v>1096</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="11">
         <f t="shared" si="1"/>
         <v>0.202812731310141</v>
       </c>
@@ -2136,7 +2160,7 @@
         <f>N17-H17</f>
         <v>1096</v>
       </c>
-      <c r="P17" s="14">
+      <c r="P17" s="11">
         <f>O17/H17</f>
         <v>0.202812731310141</v>
       </c>
@@ -2170,7 +2194,7 @@
         <f t="shared" si="0"/>
         <v>1086.5</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="11">
         <f t="shared" si="1"/>
         <v>0.200701948831625</v>
       </c>
@@ -2179,7 +2203,7 @@
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
-      <c r="P18" s="15"/>
+      <c r="P18" s="12"/>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="7">
@@ -2210,7 +2234,7 @@
         <f t="shared" si="0"/>
         <v>860.1</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="11">
         <f t="shared" si="1"/>
         <v>0.152502703948652</v>
       </c>
@@ -2219,7 +2243,7 @@
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
-      <c r="P19" s="15"/>
+      <c r="P19" s="12"/>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="7">
@@ -2250,7 +2274,7 @@
         <f t="shared" si="0"/>
         <v>1084</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="11">
         <f t="shared" si="1"/>
         <v>0.200147710487445</v>
       </c>
@@ -2259,7 +2283,7 @@
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
-      <c r="P20" s="15"/>
+      <c r="P20" s="12"/>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="5">
@@ -2290,7 +2314,7 @@
         <f t="shared" si="0"/>
         <v>1116.7</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="11">
         <f t="shared" si="1"/>
         <v>0.207437816952427</v>
       </c>
@@ -2310,7 +2334,7 @@
         <f>N21-H21</f>
         <v>1116.7</v>
       </c>
-      <c r="P21" s="14">
+      <c r="P21" s="11">
         <f>O17/H17</f>
         <v>0.202812731310141</v>
       </c>
@@ -2344,7 +2368,7 @@
         <f t="shared" si="0"/>
         <v>875</v>
       </c>
-      <c r="J22" s="14">
+      <c r="J22" s="11">
         <f t="shared" si="1"/>
         <v>0.155400017404802</v>
       </c>
@@ -2353,7 +2377,7 @@
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
-      <c r="P22" s="15"/>
+      <c r="P22" s="12"/>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="7">
@@ -2384,7 +2408,7 @@
         <f t="shared" si="0"/>
         <v>995</v>
       </c>
-      <c r="J23" s="14">
+      <c r="J23" s="11">
         <f t="shared" si="1"/>
         <v>0.180872916325826</v>
       </c>
@@ -2393,7 +2417,7 @@
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
-      <c r="P23" s="15"/>
+      <c r="P23" s="12"/>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="7">
@@ -2424,7 +2448,7 @@
         <f t="shared" si="0"/>
         <v>764</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="11">
         <f t="shared" si="1"/>
         <v>0.133167164881518</v>
       </c>
@@ -2433,7 +2457,7 @@
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
-      <c r="P24" s="15"/>
+      <c r="P24" s="12"/>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="7">
@@ -2464,7 +2488,7 @@
         <f t="shared" si="0"/>
         <v>870</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25" s="11">
         <f t="shared" si="1"/>
         <v>0.154374932350066</v>
       </c>
@@ -2473,7 +2497,7 @@
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
-      <c r="P25" s="15"/>
+      <c r="P25" s="12"/>
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="7">
@@ -2504,7 +2528,7 @@
         <f t="shared" si="0"/>
         <v>1125</v>
       </c>
-      <c r="J26" s="14">
+      <c r="J26" s="11">
         <f t="shared" si="1"/>
         <v>0.209302325581395</v>
       </c>
@@ -2513,7 +2537,7 @@
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
-      <c r="P26" s="15"/>
+      <c r="P26" s="12"/>
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="7">
@@ -2544,7 +2568,7 @@
         <f t="shared" si="0"/>
         <v>1100.5</v>
       </c>
-      <c r="J27" s="14">
+      <c r="J27" s="11">
         <f t="shared" si="1"/>
         <v>0.203774409415285</v>
       </c>
@@ -2553,7 +2577,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
-      <c r="P27" s="15"/>
+      <c r="P27" s="12"/>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="5">
@@ -2584,7 +2608,7 @@
         <f t="shared" si="0"/>
         <v>950.15</v>
       </c>
-      <c r="J28" s="14">
+      <c r="J28" s="11">
         <f t="shared" si="1"/>
         <v>0.171202825301585</v>
       </c>
@@ -2604,7 +2628,7 @@
         <f>N28-H28</f>
         <v>1200.15</v>
       </c>
-      <c r="P28" s="14">
+      <c r="P28" s="11">
         <f>O28/H28</f>
         <v>0.216249087813184</v>
       </c>
@@ -2638,7 +2662,7 @@
         <f t="shared" si="0"/>
         <v>1156.45</v>
       </c>
-      <c r="J29" s="14">
+      <c r="J29" s="11">
         <f t="shared" si="1"/>
         <v>0.216419795828616</v>
       </c>
@@ -2647,7 +2671,7 @@
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
-      <c r="P29" s="15"/>
+      <c r="P29" s="12"/>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="7">
@@ -2678,7 +2702,7 @@
         <f t="shared" si="0"/>
         <v>828.35</v>
       </c>
-      <c r="J30" s="14">
+      <c r="J30" s="11">
         <f t="shared" si="1"/>
         <v>0.14605097282096</v>
       </c>
@@ -2687,47 +2711,61 @@
       <c r="M30" s="7"/>
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
-      <c r="P30" s="15"/>
+      <c r="P30" s="12"/>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="7">
+      <c r="A31" s="5">
         <v>128082</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="6">
         <v>20201026</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="5">
         <v>113.259</v>
       </c>
-      <c r="G31" s="7">
-        <v>50</v>
-      </c>
-      <c r="H31" s="7">
+      <c r="G31" s="5">
+        <v>50</v>
+      </c>
+      <c r="H31" s="5">
         <v>5662.95</v>
       </c>
-      <c r="I31" s="7">
-        <f>(130-F31)*G31</f>
+      <c r="I31" s="5">
+        <f t="shared" si="0"/>
         <v>837.05</v>
       </c>
-      <c r="J31" s="14">
-        <f>I31/H31</f>
+      <c r="J31" s="11">
+        <f t="shared" si="1"/>
         <v>0.147811652937073</v>
       </c>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="15"/>
+      <c r="K31" s="5">
+        <v>20201126</v>
+      </c>
+      <c r="L31" s="5">
+        <v>131</v>
+      </c>
+      <c r="M31" s="5">
+        <v>50</v>
+      </c>
+      <c r="N31" s="5">
+        <v>6550</v>
+      </c>
+      <c r="O31" s="5">
+        <f>N31-H31</f>
+        <v>887.05</v>
+      </c>
+      <c r="P31" s="11">
+        <f>O31/H31</f>
+        <v>0.156640973344282</v>
+      </c>
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="7">
@@ -2755,11 +2793,11 @@
         <v>5492</v>
       </c>
       <c r="I32" s="7">
-        <f>(130-F32)*G32</f>
+        <f t="shared" si="0"/>
         <v>1008</v>
       </c>
-      <c r="J32" s="14">
-        <f>I32/H32</f>
+      <c r="J32" s="11">
+        <f t="shared" si="1"/>
         <v>0.18353969410051</v>
       </c>
       <c r="K32" s="7"/>
@@ -2767,7 +2805,7 @@
       <c r="M32" s="7"/>
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
-      <c r="P32" s="15"/>
+      <c r="P32" s="12"/>
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="7">
@@ -2795,11 +2833,11 @@
         <v>5575.5</v>
       </c>
       <c r="I33" s="7">
-        <f>(130-F33)*G33</f>
+        <f t="shared" si="0"/>
         <v>924.5</v>
       </c>
-      <c r="J33" s="14">
-        <f>I33/H33</f>
+      <c r="J33" s="11">
+        <f t="shared" si="1"/>
         <v>0.165814725136759</v>
       </c>
       <c r="K33" s="7"/>
@@ -2807,313 +2845,462 @@
       <c r="M33" s="7"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
-      <c r="P33" s="15"/>
+      <c r="P33" s="12"/>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="9">
+      <c r="A34" s="5">
         <v>128094</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="6">
         <v>20201026</v>
       </c>
-      <c r="F34" s="9">
+      <c r="F34" s="5">
         <v>114.81</v>
       </c>
-      <c r="G34" s="9">
-        <v>50</v>
-      </c>
-      <c r="H34" s="9">
+      <c r="G34" s="5">
+        <v>50</v>
+      </c>
+      <c r="H34" s="5">
         <v>5470.5</v>
       </c>
       <c r="I34" s="5">
-        <f>(130-F34)*G34</f>
+        <f t="shared" si="0"/>
         <v>759.5</v>
       </c>
-      <c r="J34" s="14">
-        <f>I34/H34</f>
+      <c r="J34" s="11">
+        <f t="shared" si="1"/>
         <v>0.138835572616763</v>
       </c>
-      <c r="K34" s="9">
+      <c r="K34" s="5">
         <v>20201027</v>
       </c>
-      <c r="L34" s="9">
+      <c r="L34" s="5">
         <v>130.417</v>
       </c>
-      <c r="M34" s="9">
-        <v>50</v>
-      </c>
-      <c r="N34" s="9">
+      <c r="M34" s="5">
+        <v>50</v>
+      </c>
+      <c r="N34" s="5">
         <v>6520.85</v>
       </c>
-      <c r="O34" s="9">
+      <c r="O34" s="5">
         <f>N34-H34</f>
         <v>1050.35</v>
       </c>
-      <c r="P34" s="16">
+      <c r="P34" s="11">
         <f>O34/H34</f>
         <v>0.192002559181062</v>
       </c>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="17"/>
+      <c r="A35" s="7">
+        <v>128094</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="8">
+        <v>20201111</v>
+      </c>
+      <c r="F35" s="7">
+        <v>111.586</v>
+      </c>
+      <c r="G35" s="7">
+        <v>50</v>
+      </c>
+      <c r="H35" s="7">
+        <v>5579.3</v>
+      </c>
+      <c r="I35" s="7">
+        <f t="shared" si="0"/>
+        <v>920.7</v>
+      </c>
+      <c r="J35" s="11">
+        <f t="shared" si="1"/>
+        <v>0.165020701521696</v>
+      </c>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="12"/>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="17"/>
+      <c r="A36" s="7">
+        <v>128018</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="8">
+        <v>20201116</v>
+      </c>
+      <c r="F36" s="7">
+        <v>107.281</v>
+      </c>
+      <c r="G36" s="7">
+        <v>50</v>
+      </c>
+      <c r="H36" s="7">
+        <v>5364.05</v>
+      </c>
+      <c r="I36" s="7">
+        <f t="shared" si="0"/>
+        <v>1135.95</v>
+      </c>
+      <c r="J36" s="11">
+        <f t="shared" si="1"/>
+        <v>0.211770956646564</v>
+      </c>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="12"/>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="17"/>
+      <c r="A37" s="7">
+        <v>128093</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="8">
+        <v>20201123</v>
+      </c>
+      <c r="F37" s="7">
+        <v>111.14</v>
+      </c>
+      <c r="G37" s="7">
+        <v>50</v>
+      </c>
+      <c r="H37" s="7">
+        <v>5557</v>
+      </c>
+      <c r="I37" s="7">
+        <f t="shared" si="0"/>
+        <v>943</v>
+      </c>
+      <c r="J37" s="11">
+        <f t="shared" si="1"/>
+        <v>0.169695879071441</v>
+      </c>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="12"/>
     </row>
     <row r="38" spans="1:16">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="17"/>
+      <c r="A38" s="7">
+        <v>113033</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E38" s="8">
+        <v>20201140</v>
+      </c>
+      <c r="F38" s="7">
+        <v>109.464</v>
+      </c>
+      <c r="G38" s="7">
+        <v>50</v>
+      </c>
+      <c r="H38" s="7">
+        <v>5473.2</v>
+      </c>
+      <c r="I38" s="7">
+        <f t="shared" si="0"/>
+        <v>1026.8</v>
+      </c>
+      <c r="J38" s="11">
+        <f t="shared" si="1"/>
+        <v>0.18760505737046</v>
+      </c>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="12"/>
     </row>
     <row r="39" spans="1:16">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="17"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="17"/>
+      <c r="A39" s="7">
+        <v>128082</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" s="1">
+        <v>20201207</v>
+      </c>
+      <c r="F39" s="9">
+        <v>114.589</v>
+      </c>
+      <c r="G39" s="9">
+        <v>50</v>
+      </c>
+      <c r="H39" s="9">
+        <f>G39*F39</f>
+        <v>5729.45</v>
+      </c>
+      <c r="I39" s="7">
+        <f>(130-F39)*G39</f>
+        <v>770.55</v>
+      </c>
+      <c r="J39" s="11">
+        <f>I39/H39</f>
+        <v>0.134489348890382</v>
+      </c>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="12"/>
     </row>
     <row r="40" spans="1:16">
-      <c r="A40" s="11"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="17"/>
+      <c r="A40" s="7">
+        <v>128026</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" s="8">
+        <v>20201215</v>
+      </c>
+      <c r="F40" s="7">
+        <v>103.998</v>
+      </c>
+      <c r="G40" s="7">
+        <v>50</v>
+      </c>
+      <c r="H40" s="7">
+        <v>5199.9</v>
+      </c>
+      <c r="I40" s="7">
+        <f>(130-F40)*G40</f>
+        <v>1300.1</v>
+      </c>
+      <c r="J40" s="11">
+        <f>I40/H40</f>
+        <v>0.250024038923825</v>
+      </c>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="12"/>
     </row>
     <row r="41" spans="1:16">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="17"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="17"/>
+      <c r="A41" s="7">
+        <v>113542</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="8">
+        <v>20201221</v>
+      </c>
+      <c r="F41" s="7">
+        <v>114.69</v>
+      </c>
+      <c r="G41" s="7">
+        <v>50</v>
+      </c>
+      <c r="H41" s="7">
+        <v>5734.5</v>
+      </c>
+      <c r="I41" s="7">
+        <f>(130-F41)*G41</f>
+        <v>765.5</v>
+      </c>
+      <c r="J41" s="11">
+        <f>I41/H41</f>
+        <v>0.133490278141076</v>
+      </c>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="12"/>
     </row>
     <row r="42" spans="1:16">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="17"/>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="17"/>
+      <c r="A42" s="7">
+        <v>123049</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" s="8">
+        <v>20210104</v>
+      </c>
+      <c r="F42" s="7">
+        <v>111</v>
+      </c>
+      <c r="G42" s="7">
+        <v>20</v>
+      </c>
+      <c r="H42" s="7">
+        <v>2220</v>
+      </c>
+      <c r="I42" s="7">
+        <f>(130-F42)*G42</f>
+        <v>380</v>
+      </c>
+      <c r="J42" s="11">
+        <f>I42/H42</f>
+        <v>0.171171171171171</v>
+      </c>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="12"/>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="17"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="17"/>
+      <c r="A43" s="7">
+        <v>128105</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43" s="8">
+        <v>20210104</v>
+      </c>
+      <c r="F43" s="7">
+        <v>107.988</v>
+      </c>
+      <c r="G43" s="7">
+        <v>30</v>
+      </c>
+      <c r="H43" s="7">
+        <v>3239.64</v>
+      </c>
+      <c r="I43" s="7">
+        <f>(130-F43)*G43</f>
+        <v>660.36</v>
+      </c>
+      <c r="J43" s="11">
+        <f>I43/H43</f>
+        <v>0.203837463421862</v>
+      </c>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="12"/>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="17"/>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
-      <c r="P44" s="17"/>
-    </row>
-    <row r="45" spans="1:16">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="17"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="17"/>
-    </row>
-    <row r="46" spans="1:16">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="17"/>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="17"/>
-    </row>
-    <row r="47" spans="1:16">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="17"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="17"/>
-    </row>
-    <row r="48" spans="1:16">
-      <c r="A48" s="11"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="17"/>
-      <c r="K48" s="11"/>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
-      <c r="O48" s="11"/>
-      <c r="P48" s="17"/>
+      <c r="A44" s="7">
+        <v>110060</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E44" s="8">
+        <v>20210104</v>
+      </c>
+      <c r="F44" s="7">
+        <v>110.6</v>
+      </c>
+      <c r="G44" s="7">
+        <v>30</v>
+      </c>
+      <c r="H44" s="7">
+        <v>3318</v>
+      </c>
+      <c r="I44" s="7">
+        <f>(130-F44)*G44</f>
+        <v>582</v>
+      </c>
+      <c r="J44" s="11">
+        <f>I44/H44</f>
+        <v>0.175406871609403</v>
+      </c>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>